<commit_message>
Fixed gitignore which had an invalid name, updated Alphas_Cronbach.xlsx, with values for GRIT-O and GRIT-S scales. Finally, ensured that alphas for GRIT-S are calculated in cfa.r.
</commit_message>
<xml_diff>
--- a/XLSX/Alphas_Cronbach.xlsx
+++ b/XLSX/Alphas_Cronbach.xlsx
@@ -1,20 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0964EDCB-847B-41AA-BF14-E731A57C8E39}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calvarezg/Code/sjaltermatt/memoria-uandes/XLSX/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EO" sheetId="1" r:id="rId1"/>
     <sheet name="SGS" sheetId="2" r:id="rId2"/>
     <sheet name="RITI" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Factor</t>
   </si>
@@ -76,12 +86,18 @@
   </si>
   <si>
     <t>Incremental Beliefs (Self)</t>
+  </si>
+  <si>
+    <t>Grit-O</t>
+  </si>
+  <si>
+    <t>Grit-S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,13 +133,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,20 +423,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -445,7 +462,7 @@
         <v>0.56799999999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -459,7 +476,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -473,7 +490,7 @@
         <v>0.65500000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -487,7 +504,7 @@
         <v>0.79200000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -501,7 +518,7 @@
         <v>0.48299999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -515,7 +532,7 @@
         <v>0.65100000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -529,7 +546,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -543,61 +560,52 @@
         <v>0.61799999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D2745D-8BEF-4DB9-9B32-777B1ADC48FB}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>12</v>
-      </c>
-      <c r="B2">
-        <v>188</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
       </c>
       <c r="B3">
         <v>188</v>
@@ -606,31 +614,95 @@
         <v>6</v>
       </c>
       <c r="D3">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>188</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
         <v>0.622</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>188</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>0.67400000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>188</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>0.60399999999999998</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF81411B-BF2E-4313-9D11-21E2D930B5B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -644,7 +716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -658,7 +730,7 @@
         <v>0.90400000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -672,7 +744,7 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -686,7 +758,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>